<commit_message>
updating car dragging game with correct layout
</commit_message>
<xml_diff>
--- a/car_emissions_database.xlsx
+++ b/car_emissions_database.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="car_emissions_database xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2617,10 +2617,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2643,13 +2659,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2981,8 +3001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F798"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A590" workbookViewId="0">
+      <selection activeCell="B600" sqref="B600"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18949,6 +18969,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>